<commit_message>
initial version with clustering, aggregated and extreme periods
</commit_message>
<xml_diff>
--- a/aggregated_single/results.xlsx
+++ b/aggregated_single/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,19 +472,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>9174000</v>
+        <v>13492947.6276</v>
       </c>
       <c r="C2" t="n">
-        <v>278000</v>
+        <v>530225.1314000001</v>
       </c>
       <c r="D2" t="n">
-        <v>834000</v>
+        <v>255848.158</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>5560</v>
+        <v>3188</v>
       </c>
     </row>
     <row r="3">
@@ -494,19 +494,41 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>13950000</v>
+        <v>10430611.779336</v>
       </c>
       <c r="C3" t="n">
-        <v>450000</v>
+        <v>329870.800764</v>
       </c>
       <c r="D3" t="n">
-        <v>1050000</v>
+        <v>837904.187</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>3000</v>
+        <v>2447</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>bs3</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>37775685.81309601</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1542039.631629</v>
+      </c>
+      <c r="D4" t="n">
+        <v>255578.218</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>3101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added elbow and silhouette applied to model's data
</commit_message>
<xml_diff>
--- a/aggregated_single/results.xlsx
+++ b/aggregated_single/results.xlsx
@@ -472,10 +472,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>13492935.61956517</v>
+        <v>13492935.61956521</v>
       </c>
       <c r="C2" t="n">
-        <v>530224.5593651686</v>
+        <v>530224.55936517</v>
       </c>
       <c r="D2" t="n">
         <v>255848.7316003759</v>
@@ -494,13 +494,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>10430607.9622327</v>
+        <v>10430607.96223269</v>
       </c>
       <c r="C3" t="n">
-        <v>329870.6190188184</v>
+        <v>329870.6190188181</v>
       </c>
       <c r="D3" t="n">
-        <v>837904.3685936861</v>
+        <v>837904.3685936857</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -516,7 +516,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>37775695.75251231</v>
+        <v>37775695.7525123</v>
       </c>
       <c r="C4" t="n">
         <v>1542040.104714323</v>

</xml_diff>

<commit_message>
initial version of aggregated using network
</commit_message>
<xml_diff>
--- a/aggregated_single/results.xlsx
+++ b/aggregated_single/results.xlsx
@@ -472,10 +472,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>13492935.61956521</v>
+        <v>13492935.61956518</v>
       </c>
       <c r="C2" t="n">
-        <v>530224.55936517</v>
+        <v>530224.559365169</v>
       </c>
       <c r="D2" t="n">
         <v>255848.7316003759</v>
@@ -494,13 +494,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>10430607.96223269</v>
+        <v>10430607.9622327</v>
       </c>
       <c r="C3" t="n">
-        <v>329870.6190188181</v>
+        <v>329870.6190188184</v>
       </c>
       <c r="D3" t="n">
-        <v>837904.3685936857</v>
+        <v>837904.3685936861</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -516,7 +516,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>37775695.7525123</v>
+        <v>37775695.75251231</v>
       </c>
       <c r="C4" t="n">
         <v>1542040.104714323</v>

</xml_diff>